<commit_message>
Removing number of peaks
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCLA\Winter 18\CS205\Activity_Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92975C06-950F-4E64-9AE2-6D97BA99C7D3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420254E5-31A5-4ED3-9EC5-9E626F632454}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" activeTab="1" xr2:uid="{67DE40E5-A26B-486F-8568-103A94EB6ADC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Mean</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Accelerometer +  Gyroscope</t>
   </si>
   <si>
-    <t>Number of peaks</t>
-  </si>
-  <si>
     <t>0-2</t>
   </si>
   <si>
@@ -106,27 +103,18 @@
     <t>41-43</t>
   </si>
   <si>
-    <t>44-46</t>
-  </si>
-  <si>
     <t>0-2, 3-5, 6-8, 9-11</t>
   </si>
   <si>
     <t>0-2, 3-5, 6-8, , 9-11, 12, 29-31, 32-34</t>
   </si>
   <si>
-    <t>0-2, 3-5, 6-8, 9-11, 13-25, 44-46</t>
-  </si>
-  <si>
     <t>0-2, 3-5, 6-8, 9-11, 26-28, 35-37</t>
   </si>
   <si>
     <t>0-2, 3-5, 6-8, 9-11, 38-40, 41-43</t>
   </si>
   <si>
-    <t>0-46</t>
-  </si>
-  <si>
     <t>Accelerometer only</t>
   </si>
   <si>
@@ -137,6 +125,12 @@
   </si>
   <si>
     <t>LSTM accerlerometer and gyroscope</t>
+  </si>
+  <si>
+    <t>0-2, 3-5, 6-8, 9-11, 13-25</t>
+  </si>
+  <si>
+    <t>0-43</t>
   </si>
 </sst>
 </file>
@@ -500,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6386834-260F-4325-B8B4-225078D18DF7}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,12 +506,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -525,7 +519,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -533,7 +527,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -541,7 +535,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -557,7 +551,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -565,7 +559,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -573,7 +567,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -581,7 +575,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -589,7 +583,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -597,7 +591,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -605,18 +599,10 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -626,32 +612,32 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -659,17 +645,17 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +669,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,12 +680,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -707,7 +693,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -715,7 +701,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -723,7 +709,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -739,7 +725,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -747,7 +733,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -755,7 +741,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -763,7 +749,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -771,7 +757,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -779,7 +765,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -787,18 +773,10 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -808,32 +786,32 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -841,17 +819,17 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>